<commit_message>
Test Result Graphs added
</commit_message>
<xml_diff>
--- a/Kinematic Analysis/PRBM - Force_Deflection_Data.xlsx
+++ b/Kinematic Analysis/PRBM - Force_Deflection_Data.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="104" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="124" uniqueCount="4">
   <si>
     <t>Deflection_S1_mm</t>
   </si>
@@ -77,7 +77,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="16.44140625" customWidth="true"/>
-    <col min="2" max="2" width="15.21875" customWidth="true"/>
+    <col min="2" max="2" width="15.88671875" customWidth="true"/>
     <col min="3" max="3" width="11.5546875" customWidth="true"/>
     <col min="4" max="4" width="11.5546875" customWidth="true"/>
   </cols>
@@ -101,7 +101,7 @@
         <v>-0</v>
       </c>
       <c r="B2" s="0">
-        <v>1.0718718342801773e-18</v>
+        <v>-5.7285632743367718e-17</v>
       </c>
       <c r="C2" s="0">
         <v>18.000000000000014</v>
@@ -115,41 +115,41 @@
         <v>2.2222222222222285</v>
       </c>
       <c r="B3" s="0">
-        <v>0.70589886740542085</v>
+        <v>10.81083988149755</v>
       </c>
       <c r="C3" s="0">
-        <v>21.746174182750178</v>
+        <v>19.957610052965681</v>
       </c>
       <c r="D3" s="0">
-        <v>338.25382581724983</v>
+        <v>340.04238994703434</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0">
-        <v>4.4444444444444429</v>
+        <v>4.4444444444444571</v>
       </c>
       <c r="B4" s="0">
-        <v>1.151303648177916</v>
+        <v>19.059269419946361</v>
       </c>
       <c r="C4" s="0">
-        <v>24.958715183094913</v>
+        <v>21.746174182750178</v>
       </c>
       <c r="D4" s="0">
-        <v>335.04128481690509</v>
+        <v>338.25382581724983</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0">
-        <v>6.6666666666666714</v>
+        <v>6.6666666666666572</v>
       </c>
       <c r="B5" s="0">
-        <v>1.4693286723691861</v>
+        <v>25.646483063593774</v>
       </c>
       <c r="C5" s="0">
-        <v>27.823470735194409</v>
+        <v>23.404535767535407</v>
       </c>
       <c r="D5" s="0">
-        <v>332.17652926480559</v>
+        <v>336.59546423246462</v>
       </c>
     </row>
     <row r="6">
@@ -157,13 +157,13 @@
         <v>8.8888888888888857</v>
       </c>
       <c r="B6" s="0">
-        <v>1.7141283418147817</v>
+        <v>31.085198500803735</v>
       </c>
       <c r="C6" s="0">
-        <v>30.439157851663541</v>
+        <v>24.958715183094913</v>
       </c>
       <c r="D6" s="0">
-        <v>329.56084214833646</v>
+        <v>335.04128481690509</v>
       </c>
     </row>
     <row r="7">
@@ -171,55 +171,55 @@
         <v>11.111111111111114</v>
       </c>
       <c r="B7" s="0">
-        <v>1.9124257161267804</v>
+        <v>35.691412082395445</v>
       </c>
       <c r="C7" s="0">
-        <v>32.865645007260206</v>
+        <v>26.427150708304854</v>
       </c>
       <c r="D7" s="0">
-        <v>327.13435499273976</v>
+        <v>333.57284929169515</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0">
-        <v>13.333333333333329</v>
+        <v>13.333333333333343</v>
       </c>
       <c r="B8" s="0">
-        <v>2.0791288179404619</v>
+        <v>39.671874153968027</v>
       </c>
       <c r="C8" s="0">
-        <v>35.142479165645554</v>
+        <v>27.823470735194409</v>
       </c>
       <c r="D8" s="0">
-        <v>324.85752083435449</v>
+        <v>332.17652926480559</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0">
-        <v>15.555555555555557</v>
+        <v>15.555555555555543</v>
       </c>
       <c r="B9" s="0">
-        <v>2.2232983195918519</v>
+        <v>43.168290266053326</v>
       </c>
       <c r="C9" s="0">
-        <v>37.29740171877971</v>
+        <v>29.158085140248303</v>
       </c>
       <c r="D9" s="0">
-        <v>322.70259828122028</v>
+        <v>330.84191485975174</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0">
-        <v>17.777777777777786</v>
+        <v>17.777777777777771</v>
       </c>
       <c r="B10" s="0">
-        <v>2.3508024659194993</v>
+        <v>46.28146522899911</v>
       </c>
       <c r="C10" s="0">
-        <v>39.35076334666666</v>
+        <v>30.439157851663541</v>
       </c>
       <c r="D10" s="0">
-        <v>320.64923665333333</v>
+        <v>329.56084214833646</v>
       </c>
     </row>
     <row r="11">
@@ -227,13 +227,13 @@
         <v>20</v>
       </c>
       <c r="B11" s="0">
-        <v>2.4656337881107806</v>
+        <v>49.085327854699514</v>
       </c>
       <c r="C11" s="0">
-        <v>41.318020349965309</v>
+        <v>31.673231479421272</v>
       </c>
       <c r="D11" s="0">
-        <v>318.68197965003475</v>
+        <v>328.3267685205787</v>
       </c>
     </row>
   </sheetData>

</xml_diff>